<commit_message>
Documentación de la Aplicación - Añadida parte de Miguel
</commit_message>
<xml_diff>
--- a/sdi1920-entrega2-914.xlsx
+++ b/sdi1920-entrega2-914.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\Universidad de Oviedo\ENRIQUE ANTONIO DE LA CAL MARIN - SDI\1920\prácticas_propuestas\practica2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel\git\sdi1920-entrega2-914-909\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="14_{20FCFC55-68BC-458D-A929-FD17B87A842E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{5711F26F-3BCC-4857-AAA8-F0BBCC476104}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE050BF-D5B3-40AD-8E14-73BA8D96817E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1490" yWindow="340" windowWidth="27780" windowHeight="16190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2930" yWindow="340" windowWidth="14400" windowHeight="7360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pruebas" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="127">
   <si>
     <t>Puntuación (Para rellenar por el profesor)</t>
   </si>
@@ -404,6 +406,72 @@
   </si>
   <si>
     <t>[Prueba31] Identificarse con un usuario A que al menos tenga 3 amigos, ir al chat del ultimo amigo de la lista y enviarle un mensaje, volver a la lista de amigos y comprobar que el usuario al que se le ha enviado el mensaje esta en primera posición. Identificarse con el usuario B y enviarle un mensaje al usuario A. Volver a identificarse con el usuario A y ver que el usuario que acaba de mandarle el mensaje es el primero en su lista de amigos.</t>
+  </si>
+  <si>
+    <t>Se reliza un registro estándar completando todos los campos y con un email no presente en la base de datos, este email será usado en posteriores pruebas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se realiza un registro en el que se intercalaran  un campo vacio en cada interaccion y sen intentará aceptar, la última es con todos ellos vacios </t>
+  </si>
+  <si>
+    <t>Se reliza un registro estándar completando todos los campos pero con el campo de confirmacion de contraseña erroneo, se espera mensaje de error concreto.</t>
+  </si>
+  <si>
+    <t>Se realiza un registro estándar pero con un email que ya se encuentre en la base de datos, se espera mensaje de error concreto a esta falta.</t>
+  </si>
+  <si>
+    <t>Se realiza un inicio de sesion con el usuario introducido en la primera prueba, se comprueba que nos dirige a la vista de lista de usuarios</t>
+  </si>
+  <si>
+    <t>Se realiza un inicio de sesion con una cuenta existente pero una contraseña erronea, se espera mensaje de error para email o contraseña erroneo.</t>
+  </si>
+  <si>
+    <t>Se inicia sesión con un usuario, se comprueba que el botón de cerrar sesión es visible, se cierra la sesión y se comprueba que el botón no es visible para el usuario.</t>
+  </si>
+  <si>
+    <t>Se inicia sesión y se hace una busqueda vacia en la vista de usuarios, se comprueba que aparece toda la primera página de usuarios</t>
+  </si>
+  <si>
+    <t>Se inicia sesión y se hace una busqueda con un nombre inexistente en la base de datos en la vista de usuarios, se comprueba que no aparece ningún usuario.</t>
+  </si>
+  <si>
+    <t>Se hacen 3 busquedas en la vista de usuarios, una con un email de usuario, otra por nombre y otra por apellido, se comprueba que devuelve al usuario correspondiente</t>
+  </si>
+  <si>
+    <t>Se inicia sesión y con un método se comprueba que se encuentran los 11 usuarios en el sistema, la prueba tiene en cuenta el sistema de paginación</t>
+  </si>
+  <si>
+    <t>Se inicia sesion con un usuario de sistema, se cierra la sesion y se comprueba que volvemos a la ventana de identificación</t>
+  </si>
+  <si>
+    <t>Se realiza un inicio de sesion con una cuenta inexistente, se espera mensaje de error para email o contraseña erróneo.</t>
+  </si>
+  <si>
+    <t>Se realiza un inicio de sesion sin completar los campos del formulario, se comprueba que seguimos en la vista de Identificación</t>
+  </si>
+  <si>
+    <t>Se inicia sesion con el usuario de la primera prueba y se manda una solicitud de amistad al usuario 0, se cierra sesión, se identifica como este usuario y comprobamos que aparece la solicitud en la vista de solicitudes</t>
+  </si>
+  <si>
+    <t>Con el usuario de la prueba uno se repite el procedimiento de la prueba 15, al enviar la solicitud comprobamos que salta un mensaje de error correspondiente al problema</t>
+  </si>
+  <si>
+    <t>Se inicia sesión con el usuario 3 y se comprueba que tiene 5 invitaciones de amistad</t>
+  </si>
+  <si>
+    <t>Se inicia sesión con el usuario 0 y se acepta la amistad enviada en la prueba 15, se comprueba que sale mensaje de confirmación,  se comprueba que aparece la amistad  en amigos pero no en solicitudes de amistad.</t>
+  </si>
+  <si>
+    <t>Se inicia sesión con usuario 0 y se comprueba que aparece la amistad que corresponde</t>
+  </si>
+  <si>
+    <t>Se intenta navegar directamente a la vista de listado de usuarios, se comprueba que nos dirige a la vista de identificación</t>
+  </si>
+  <si>
+    <t>Se intenta navegar directamente a la vista de solicitudes de amistad, se comprueba que nos dirige a la vista de identificación</t>
+  </si>
+  <si>
+    <t>Se intenta navegar directamente a la vista de lista de amigos, se comprueba que nos dirige a la vista de identificación</t>
   </si>
 </sst>
 </file>
@@ -790,6 +858,25 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -839,25 +926,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1140,8 +1208,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I96" sqref="I96"/>
+    <sheetView tabSelected="1" topLeftCell="D70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F88" sqref="F88:H88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1155,96 +1223,96 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="2" spans="1:9" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="32"/>
+      <c r="B2" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:9" ht="21" x14ac:dyDescent="0.5">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
     </row>
     <row r="4" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="34">
+      <c r="B4" s="43">
         <f>H46</f>
-        <v>0</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
+        <v>4</v>
+      </c>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
     </row>
     <row r="5" spans="1:9" ht="21" x14ac:dyDescent="0.5">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
     </row>
     <row r="6" spans="1:9" ht="26" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="34">
+      <c r="B6" s="43">
         <f>H59</f>
         <v>0</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
     </row>
     <row r="7" spans="1:9" ht="26" x14ac:dyDescent="0.6">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="38" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="29"/>
-      <c r="H7" s="29"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="B8" s="35">
+      <c r="B8" s="44">
         <f>B4-B6</f>
-        <v>0</v>
-      </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
+        <v>4</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
     </row>
     <row r="10" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="11" spans="1:9" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="31"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="32"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="41"/>
     </row>
     <row r="12" spans="1:9" ht="31" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
@@ -1289,7 +1357,7 @@
       </c>
       <c r="E13" s="1">
         <f t="shared" ref="E13:E22" si="1">COUNTIFS($C$64:$C$111,$B13,$E$64:$E$111,"=OK")</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" ref="F13:F22" si="2">COUNTIFS($C$64:$C$111,$B13,$E$64:$E$111,"FAIL")</f>
@@ -1297,11 +1365,11 @@
       </c>
       <c r="G13" s="1">
         <f t="shared" ref="G13:G22" si="3">COUNTIFS($C$64:$C$111,$B13,$E$64:$E$111,"=SIN")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1">
         <f>MIN(D13,(E13/C13)*D13)</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
@@ -1320,7 +1388,7 @@
       </c>
       <c r="E14" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="2"/>
@@ -1328,11 +1396,11 @@
       </c>
       <c r="G14" s="1">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" ref="H14:H34" si="4">MIN(D14,(E14/C14)*D14)</f>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
@@ -1351,7 +1419,7 @@
       </c>
       <c r="E15" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="2"/>
@@ -1359,11 +1427,11 @@
       </c>
       <c r="G15" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
@@ -1382,7 +1450,7 @@
       </c>
       <c r="E16" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="2"/>
@@ -1390,11 +1458,11 @@
       </c>
       <c r="G16" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H16" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.35">
@@ -1413,7 +1481,7 @@
       </c>
       <c r="E17" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="2"/>
@@ -1421,11 +1489,11 @@
       </c>
       <c r="G17" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
@@ -1444,7 +1512,7 @@
       </c>
       <c r="E18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="2"/>
@@ -1452,11 +1520,11 @@
       </c>
       <c r="G18" s="1">
         <f t="shared" si="3"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1475,7 +1543,7 @@
       </c>
       <c r="E19" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="2"/>
@@ -1483,11 +1551,11 @@
       </c>
       <c r="G19" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.35">
@@ -1506,7 +1574,7 @@
       </c>
       <c r="E20" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="2"/>
@@ -1514,11 +1582,11 @@
       </c>
       <c r="G20" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.35">
@@ -1537,7 +1605,7 @@
       </c>
       <c r="E21" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="2"/>
@@ -1545,11 +1613,11 @@
       </c>
       <c r="G21" s="1">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.35">
@@ -1568,7 +1636,7 @@
       </c>
       <c r="E22" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="2"/>
@@ -1576,11 +1644,11 @@
       </c>
       <c r="G22" s="1">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.35">
@@ -1992,7 +2060,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1">
         <f>SUM(H13:H22)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -2075,10 +2143,10 @@
       <c r="H45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="21.5" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B46" s="49" t="s">
+      <c r="B46" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="50"/>
+      <c r="C46" s="28"/>
       <c r="D46" s="24">
         <f>SUM(D13:D35)</f>
         <v>11</v>
@@ -2090,35 +2158,35 @@
       </c>
       <c r="H46" s="11">
         <f>SUM(H13:H35)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I46" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="31.5" thickBot="1" x14ac:dyDescent="0.75">
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="37"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="38"/>
+      <c r="C47" s="46"/>
+      <c r="D47" s="46"/>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="47"/>
       <c r="I47" s="2"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B48" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="42" t="s">
+      <c r="C48" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="D48" s="43"/>
-      <c r="E48" s="43"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="43"/>
+      <c r="D48" s="52"/>
+      <c r="E48" s="52"/>
+      <c r="F48" s="52"/>
+      <c r="G48" s="52"/>
       <c r="H48" s="5" t="s">
         <v>18</v>
       </c>
@@ -2127,110 +2195,110 @@
       <c r="B49" s="6">
         <v>1</v>
       </c>
-      <c r="C49" s="44"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
+      <c r="C49" s="33"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B50" s="6">
         <v>2</v>
       </c>
-      <c r="C50" s="44"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="45"/>
-      <c r="G50" s="45"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
       <c r="H50" s="7"/>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B51" s="6">
         <v>3</v>
       </c>
-      <c r="C51" s="44"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="45"/>
-      <c r="G51" s="45"/>
+      <c r="C51" s="33"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
       <c r="H51" s="7"/>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B52" s="6">
         <v>4</v>
       </c>
-      <c r="C52" s="44"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="45"/>
-      <c r="G52" s="45"/>
+      <c r="C52" s="33"/>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
       <c r="H52" s="7"/>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B53" s="6">
         <v>5</v>
       </c>
-      <c r="C53" s="44"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="45"/>
-      <c r="F53" s="45"/>
-      <c r="G53" s="45"/>
+      <c r="C53" s="33"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
       <c r="H53" s="7"/>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B54" s="6">
         <v>6</v>
       </c>
-      <c r="C54" s="44"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="45"/>
-      <c r="G54" s="45"/>
+      <c r="C54" s="33"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
       <c r="H54" s="7"/>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B55" s="6">
         <v>7</v>
       </c>
-      <c r="C55" s="44"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="45"/>
-      <c r="G55" s="45"/>
+      <c r="C55" s="33"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
       <c r="H55" s="7"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B56" s="6">
         <v>8</v>
       </c>
-      <c r="C56" s="44"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="45"/>
-      <c r="G56" s="45"/>
+      <c r="C56" s="33"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
       <c r="H56" s="7"/>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B57" s="6">
         <v>9</v>
       </c>
-      <c r="C57" s="44"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="45"/>
+      <c r="C57" s="33"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="31"/>
+      <c r="G57" s="31"/>
       <c r="H57" s="7"/>
     </row>
     <row r="58" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B58" s="8">
         <v>10</v>
       </c>
-      <c r="C58" s="46"/>
-      <c r="D58" s="47"/>
-      <c r="E58" s="47"/>
-      <c r="F58" s="47"/>
-      <c r="G58" s="47"/>
+      <c r="C58" s="34"/>
+      <c r="D58" s="35"/>
+      <c r="E58" s="35"/>
+      <c r="F58" s="35"/>
+      <c r="G58" s="35"/>
       <c r="H58" s="9"/>
     </row>
     <row r="59" spans="2:11" ht="26" x14ac:dyDescent="0.6">
@@ -2269,15 +2337,15 @@
       <c r="H61" s="1"/>
     </row>
     <row r="62" spans="2:11" ht="31" x14ac:dyDescent="0.7">
-      <c r="B62" s="39" t="s">
+      <c r="B62" s="48" t="s">
         <v>21</v>
       </c>
-      <c r="C62" s="40"/>
-      <c r="D62" s="40"/>
-      <c r="E62" s="40"/>
-      <c r="F62" s="40"/>
-      <c r="G62" s="40"/>
-      <c r="H62" s="41"/>
+      <c r="C62" s="49"/>
+      <c r="D62" s="49"/>
+      <c r="E62" s="49"/>
+      <c r="F62" s="49"/>
+      <c r="G62" s="49"/>
+      <c r="H62" s="50"/>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B63" s="3" t="s">
@@ -2292,16 +2360,16 @@
       <c r="E63" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="F63" s="27" t="s">
+      <c r="F63" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="G63" s="28"/>
-      <c r="H63" s="28"/>
-      <c r="I63" s="27" t="s">
+      <c r="G63" s="37"/>
+      <c r="H63" s="37"/>
+      <c r="I63" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="J63" s="28"/>
-      <c r="K63" s="28"/>
+      <c r="J63" s="37"/>
+      <c r="K63" s="37"/>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B64" s="1">
@@ -2314,11 +2382,13 @@
         <v>25</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F64" s="45"/>
-      <c r="G64" s="48"/>
-      <c r="H64" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F64" s="31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
       <c r="I64" s="26" t="s">
         <v>74</v>
       </c>
@@ -2334,11 +2404,13 @@
         <v>25</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F65" s="45"/>
-      <c r="G65" s="48"/>
-      <c r="H65" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F65" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="G65" s="32"/>
+      <c r="H65" s="32"/>
       <c r="I65" s="26" t="s">
         <v>75</v>
       </c>
@@ -2354,11 +2426,13 @@
         <v>25</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F66" s="45"/>
-      <c r="G66" s="48"/>
-      <c r="H66" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F66" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="G66" s="32"/>
+      <c r="H66" s="32"/>
       <c r="I66" s="26" t="s">
         <v>76</v>
       </c>
@@ -2374,11 +2448,13 @@
         <v>25</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F67" s="45"/>
-      <c r="G67" s="48"/>
-      <c r="H67" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F67" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="G67" s="32"/>
+      <c r="H67" s="32"/>
       <c r="I67" s="26" t="s">
         <v>77</v>
       </c>
@@ -2394,11 +2470,13 @@
         <v>25</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F68" s="45"/>
-      <c r="G68" s="48"/>
-      <c r="H68" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F68" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="G68" s="32"/>
+      <c r="H68" s="32"/>
       <c r="I68" s="26" t="s">
         <v>78</v>
       </c>
@@ -2414,11 +2492,13 @@
         <v>25</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F69" s="45"/>
-      <c r="G69" s="48"/>
-      <c r="H69" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F69" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="G69" s="32"/>
+      <c r="H69" s="32"/>
       <c r="I69" s="26" t="s">
         <v>79</v>
       </c>
@@ -2434,11 +2514,13 @@
         <v>25</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F70" s="45"/>
-      <c r="G70" s="48"/>
-      <c r="H70" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F70" s="31" t="s">
+        <v>110</v>
+      </c>
+      <c r="G70" s="32"/>
+      <c r="H70" s="32"/>
       <c r="I70" s="26" t="s">
         <v>80</v>
       </c>
@@ -2454,11 +2536,13 @@
         <v>25</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F71" s="45"/>
-      <c r="G71" s="48"/>
-      <c r="H71" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F71" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="G71" s="32"/>
+      <c r="H71" s="32"/>
       <c r="I71" s="26" t="s">
         <v>81</v>
       </c>
@@ -2474,11 +2558,13 @@
         <v>25</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F72" s="45"/>
-      <c r="G72" s="48"/>
-      <c r="H72" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F72" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="G72" s="32"/>
+      <c r="H72" s="32"/>
       <c r="I72" s="26" t="s">
         <v>82</v>
       </c>
@@ -2494,11 +2580,13 @@
         <v>25</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F73" s="45"/>
-      <c r="G73" s="48"/>
-      <c r="H73" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F73" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="G73" s="32"/>
+      <c r="H73" s="32"/>
       <c r="I73" s="26" t="s">
         <v>83</v>
       </c>
@@ -2514,11 +2602,13 @@
         <v>25</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F74" s="45"/>
-      <c r="G74" s="48"/>
-      <c r="H74" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F74" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="G74" s="32"/>
+      <c r="H74" s="32"/>
       <c r="I74" s="26" t="s">
         <v>84</v>
       </c>
@@ -2534,11 +2624,13 @@
         <v>25</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F75" s="45"/>
-      <c r="G75" s="48"/>
-      <c r="H75" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F75" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="G75" s="32"/>
+      <c r="H75" s="32"/>
       <c r="I75" s="26" t="s">
         <v>85</v>
       </c>
@@ -2554,11 +2646,13 @@
         <v>25</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F76" s="45"/>
-      <c r="G76" s="48"/>
-      <c r="H76" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F76" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="G76" s="32"/>
+      <c r="H76" s="32"/>
       <c r="I76" s="26" t="s">
         <v>86</v>
       </c>
@@ -2574,11 +2668,13 @@
         <v>25</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F77" s="45"/>
-      <c r="G77" s="48"/>
-      <c r="H77" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F77" s="31" t="s">
+        <v>114</v>
+      </c>
+      <c r="G77" s="32"/>
+      <c r="H77" s="32"/>
       <c r="I77" s="26" t="s">
         <v>87</v>
       </c>
@@ -2594,11 +2690,13 @@
         <v>25</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F78" s="45"/>
-      <c r="G78" s="48"/>
-      <c r="H78" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F78" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="G78" s="32"/>
+      <c r="H78" s="32"/>
       <c r="I78" s="26" t="s">
         <v>88</v>
       </c>
@@ -2614,11 +2712,13 @@
         <v>25</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F79" s="45"/>
-      <c r="G79" s="48"/>
-      <c r="H79" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F79" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="G79" s="32"/>
+      <c r="H79" s="32"/>
       <c r="I79" s="26" t="s">
         <v>89</v>
       </c>
@@ -2634,11 +2734,13 @@
         <v>25</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F80" s="45"/>
-      <c r="G80" s="48"/>
-      <c r="H80" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F80" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="G80" s="32"/>
+      <c r="H80" s="32"/>
       <c r="I80" s="26" t="s">
         <v>90</v>
       </c>
@@ -2654,11 +2756,13 @@
         <v>25</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F81" s="45"/>
-      <c r="G81" s="48"/>
-      <c r="H81" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F81" s="31" t="s">
+        <v>122</v>
+      </c>
+      <c r="G81" s="32"/>
+      <c r="H81" s="32"/>
       <c r="I81" s="26" t="s">
         <v>91</v>
       </c>
@@ -2674,11 +2778,13 @@
         <v>25</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F82" s="45"/>
-      <c r="G82" s="48"/>
-      <c r="H82" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F82" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="G82" s="32"/>
+      <c r="H82" s="32"/>
       <c r="I82" s="26" t="s">
         <v>92</v>
       </c>
@@ -2694,11 +2800,13 @@
         <v>25</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F83" s="45"/>
-      <c r="G83" s="48"/>
-      <c r="H83" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F83" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="G83" s="32"/>
+      <c r="H83" s="32"/>
       <c r="I83" s="26" t="s">
         <v>93</v>
       </c>
@@ -2714,11 +2822,13 @@
         <v>25</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F84" s="45"/>
-      <c r="G84" s="48"/>
-      <c r="H84" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F84" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="G84" s="32"/>
+      <c r="H84" s="32"/>
       <c r="I84" s="26" t="s">
         <v>94</v>
       </c>
@@ -2734,11 +2844,13 @@
         <v>25</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F85" s="45"/>
-      <c r="G85" s="48"/>
-      <c r="H85" s="48"/>
+        <v>37</v>
+      </c>
+      <c r="F85" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="G85" s="32"/>
+      <c r="H85" s="32"/>
       <c r="I85" s="26" t="s">
         <v>95</v>
       </c>
@@ -2756,9 +2868,9 @@
       <c r="E86" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F86" s="45"/>
-      <c r="G86" s="48"/>
-      <c r="H86" s="48"/>
+      <c r="F86" s="31"/>
+      <c r="G86" s="32"/>
+      <c r="H86" s="32"/>
       <c r="I86" s="25" t="s">
         <v>96</v>
       </c>
@@ -2776,9 +2888,9 @@
       <c r="E87" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F87" s="45"/>
-      <c r="G87" s="48"/>
-      <c r="H87" s="48"/>
+      <c r="F87" s="31"/>
+      <c r="G87" s="32"/>
+      <c r="H87" s="32"/>
       <c r="I87" s="25" t="s">
         <v>97</v>
       </c>
@@ -2796,9 +2908,9 @@
       <c r="E88" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F88" s="45"/>
-      <c r="G88" s="48"/>
-      <c r="H88" s="48"/>
+      <c r="F88" s="31"/>
+      <c r="G88" s="32"/>
+      <c r="H88" s="32"/>
       <c r="I88" s="25" t="s">
         <v>98</v>
       </c>
@@ -2816,9 +2928,9 @@
       <c r="E89" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F89" s="45"/>
-      <c r="G89" s="48"/>
-      <c r="H89" s="48"/>
+      <c r="F89" s="31"/>
+      <c r="G89" s="32"/>
+      <c r="H89" s="32"/>
       <c r="I89" s="25" t="s">
         <v>99</v>
       </c>
@@ -2836,9 +2948,9 @@
       <c r="E90" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F90" s="45"/>
-      <c r="G90" s="48"/>
-      <c r="H90" s="48"/>
+      <c r="F90" s="31"/>
+      <c r="G90" s="32"/>
+      <c r="H90" s="32"/>
       <c r="I90" s="25" t="s">
         <v>100</v>
       </c>
@@ -2856,9 +2968,9 @@
       <c r="E91" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F91" s="45"/>
-      <c r="G91" s="48"/>
-      <c r="H91" s="48"/>
+      <c r="F91" s="31"/>
+      <c r="G91" s="32"/>
+      <c r="H91" s="32"/>
       <c r="I91" s="25" t="s">
         <v>101</v>
       </c>
@@ -2876,9 +2988,9 @@
       <c r="E92" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F92" s="45"/>
-      <c r="G92" s="48"/>
-      <c r="H92" s="48"/>
+      <c r="F92" s="31"/>
+      <c r="G92" s="32"/>
+      <c r="H92" s="32"/>
       <c r="I92" s="25" t="s">
         <v>102</v>
       </c>
@@ -2896,9 +3008,9 @@
       <c r="E93" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F93" s="45"/>
-      <c r="G93" s="48"/>
-      <c r="H93" s="48"/>
+      <c r="F93" s="31"/>
+      <c r="G93" s="32"/>
+      <c r="H93" s="32"/>
       <c r="I93" s="25" t="s">
         <v>103</v>
       </c>
@@ -2916,9 +3028,9 @@
       <c r="E94" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F94" s="45"/>
-      <c r="G94" s="48"/>
-      <c r="H94" s="48"/>
+      <c r="F94" s="31"/>
+      <c r="G94" s="32"/>
+      <c r="H94" s="32"/>
       <c r="I94" s="25" t="s">
         <v>104</v>
       </c>
@@ -2934,9 +3046,9 @@
       <c r="E95" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F95" s="45"/>
-      <c r="G95" s="48"/>
-      <c r="H95" s="48"/>
+      <c r="F95" s="31"/>
+      <c r="G95" s="32"/>
+      <c r="H95" s="32"/>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B96" s="1">
@@ -2949,9 +3061,9 @@
       <c r="E96" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F96" s="45"/>
-      <c r="G96" s="48"/>
-      <c r="H96" s="48"/>
+      <c r="F96" s="31"/>
+      <c r="G96" s="32"/>
+      <c r="H96" s="32"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B97" s="1">
@@ -2964,9 +3076,9 @@
       <c r="E97" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F97" s="45"/>
-      <c r="G97" s="48"/>
-      <c r="H97" s="48"/>
+      <c r="F97" s="31"/>
+      <c r="G97" s="32"/>
+      <c r="H97" s="32"/>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B98" s="1">
@@ -2979,9 +3091,9 @@
       <c r="E98" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F98" s="45"/>
-      <c r="G98" s="48"/>
-      <c r="H98" s="48"/>
+      <c r="F98" s="31"/>
+      <c r="G98" s="32"/>
+      <c r="H98" s="32"/>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B99" s="1">
@@ -2994,9 +3106,9 @@
       <c r="E99" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F99" s="45"/>
-      <c r="G99" s="48"/>
-      <c r="H99" s="48"/>
+      <c r="F99" s="31"/>
+      <c r="G99" s="32"/>
+      <c r="H99" s="32"/>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B100" s="1">
@@ -3009,9 +3121,9 @@
       <c r="E100" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F100" s="45"/>
-      <c r="G100" s="48"/>
-      <c r="H100" s="48"/>
+      <c r="F100" s="31"/>
+      <c r="G100" s="32"/>
+      <c r="H100" s="32"/>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B101" s="1">
@@ -3024,9 +3136,9 @@
       <c r="E101" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F101" s="45"/>
-      <c r="G101" s="48"/>
-      <c r="H101" s="48"/>
+      <c r="F101" s="31"/>
+      <c r="G101" s="32"/>
+      <c r="H101" s="32"/>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B102" s="1">
@@ -3039,9 +3151,9 @@
       <c r="E102" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F102" s="45"/>
-      <c r="G102" s="48"/>
-      <c r="H102" s="48"/>
+      <c r="F102" s="31"/>
+      <c r="G102" s="32"/>
+      <c r="H102" s="32"/>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B103" s="1">
@@ -3054,84 +3166,140 @@
       <c r="E103" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F103" s="45"/>
-      <c r="G103" s="48"/>
-      <c r="H103" s="48"/>
+      <c r="F103" s="31"/>
+      <c r="G103" s="32"/>
+      <c r="H103" s="32"/>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B104" s="21"/>
       <c r="C104" s="21"/>
       <c r="D104" s="21"/>
       <c r="E104" s="21"/>
-      <c r="F104" s="51"/>
-      <c r="G104" s="52"/>
-      <c r="H104" s="52"/>
+      <c r="F104" s="29"/>
+      <c r="G104" s="30"/>
+      <c r="H104" s="30"/>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B105" s="21"/>
       <c r="C105" s="21"/>
       <c r="D105" s="21"/>
       <c r="E105" s="21"/>
-      <c r="F105" s="51"/>
-      <c r="G105" s="52"/>
-      <c r="H105" s="52"/>
+      <c r="F105" s="29"/>
+      <c r="G105" s="30"/>
+      <c r="H105" s="30"/>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B106" s="21"/>
       <c r="C106" s="21"/>
       <c r="D106" s="21"/>
       <c r="E106" s="21"/>
-      <c r="F106" s="51"/>
-      <c r="G106" s="52"/>
-      <c r="H106" s="52"/>
+      <c r="F106" s="29"/>
+      <c r="G106" s="30"/>
+      <c r="H106" s="30"/>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B107" s="21"/>
       <c r="C107" s="21"/>
       <c r="D107" s="21"/>
       <c r="E107" s="21"/>
-      <c r="F107" s="51"/>
-      <c r="G107" s="52"/>
-      <c r="H107" s="52"/>
+      <c r="F107" s="29"/>
+      <c r="G107" s="30"/>
+      <c r="H107" s="30"/>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B108" s="21"/>
       <c r="C108" s="21"/>
       <c r="D108" s="21"/>
       <c r="E108" s="21"/>
-      <c r="F108" s="51"/>
-      <c r="G108" s="52"/>
-      <c r="H108" s="52"/>
+      <c r="F108" s="29"/>
+      <c r="G108" s="30"/>
+      <c r="H108" s="30"/>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B109" s="21"/>
       <c r="C109" s="21"/>
       <c r="D109" s="21"/>
       <c r="E109" s="21"/>
-      <c r="F109" s="51"/>
-      <c r="G109" s="52"/>
-      <c r="H109" s="52"/>
+      <c r="F109" s="29"/>
+      <c r="G109" s="30"/>
+      <c r="H109" s="30"/>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B110" s="21"/>
       <c r="C110" s="21"/>
       <c r="D110" s="21"/>
       <c r="E110" s="21"/>
-      <c r="F110" s="51"/>
-      <c r="G110" s="52"/>
-      <c r="H110" s="52"/>
+      <c r="F110" s="29"/>
+      <c r="G110" s="30"/>
+      <c r="H110" s="30"/>
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B111" s="22"/>
       <c r="C111" s="21"/>
       <c r="D111" s="21"/>
       <c r="E111" s="21"/>
-      <c r="F111" s="51"/>
-      <c r="G111" s="52"/>
-      <c r="H111" s="52"/>
+      <c r="F111" s="29"/>
+      <c r="G111" s="30"/>
+      <c r="H111" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="72">
+    <mergeCell ref="I63:K63"/>
+    <mergeCell ref="B7:H7"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="F63:H63"/>
+    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B47:H47"/>
+    <mergeCell ref="B62:H62"/>
+    <mergeCell ref="C48:G48"/>
+    <mergeCell ref="C49:G49"/>
+    <mergeCell ref="C50:G50"/>
+    <mergeCell ref="C51:G51"/>
+    <mergeCell ref="C52:G52"/>
+    <mergeCell ref="C53:G53"/>
+    <mergeCell ref="C54:G54"/>
+    <mergeCell ref="C55:G55"/>
+    <mergeCell ref="C56:G56"/>
+    <mergeCell ref="C57:G57"/>
+    <mergeCell ref="C58:G58"/>
+    <mergeCell ref="F86:H86"/>
+    <mergeCell ref="F75:H75"/>
+    <mergeCell ref="F64:H64"/>
+    <mergeCell ref="F65:H65"/>
+    <mergeCell ref="F66:H66"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="F69:H69"/>
+    <mergeCell ref="F70:H70"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="F72:H72"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="F81:H81"/>
+    <mergeCell ref="F82:H82"/>
+    <mergeCell ref="F83:H83"/>
+    <mergeCell ref="F84:H84"/>
+    <mergeCell ref="F85:H85"/>
+    <mergeCell ref="F76:H76"/>
+    <mergeCell ref="F77:H77"/>
+    <mergeCell ref="F78:H78"/>
+    <mergeCell ref="F79:H79"/>
+    <mergeCell ref="F80:H80"/>
+    <mergeCell ref="F95:H95"/>
+    <mergeCell ref="F96:H96"/>
+    <mergeCell ref="F97:H97"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F87:H87"/>
+    <mergeCell ref="F90:H90"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="F92:H92"/>
+    <mergeCell ref="F93:H93"/>
+    <mergeCell ref="F94:H94"/>
     <mergeCell ref="B46:C46"/>
     <mergeCell ref="F111:H111"/>
     <mergeCell ref="F100:H100"/>
@@ -3148,62 +3316,6 @@
     <mergeCell ref="F99:H99"/>
     <mergeCell ref="F88:H88"/>
     <mergeCell ref="F89:H89"/>
-    <mergeCell ref="F95:H95"/>
-    <mergeCell ref="F96:H96"/>
-    <mergeCell ref="F97:H97"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F87:H87"/>
-    <mergeCell ref="F90:H90"/>
-    <mergeCell ref="F91:H91"/>
-    <mergeCell ref="F92:H92"/>
-    <mergeCell ref="F93:H93"/>
-    <mergeCell ref="F94:H94"/>
-    <mergeCell ref="F82:H82"/>
-    <mergeCell ref="F83:H83"/>
-    <mergeCell ref="F84:H84"/>
-    <mergeCell ref="F85:H85"/>
-    <mergeCell ref="F76:H76"/>
-    <mergeCell ref="F77:H77"/>
-    <mergeCell ref="F78:H78"/>
-    <mergeCell ref="F79:H79"/>
-    <mergeCell ref="F80:H80"/>
-    <mergeCell ref="C57:G57"/>
-    <mergeCell ref="C58:G58"/>
-    <mergeCell ref="F86:H86"/>
-    <mergeCell ref="F75:H75"/>
-    <mergeCell ref="F64:H64"/>
-    <mergeCell ref="F65:H65"/>
-    <mergeCell ref="F66:H66"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="F69:H69"/>
-    <mergeCell ref="F70:H70"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="F72:H72"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="F81:H81"/>
-    <mergeCell ref="C52:G52"/>
-    <mergeCell ref="C53:G53"/>
-    <mergeCell ref="C54:G54"/>
-    <mergeCell ref="C55:G55"/>
-    <mergeCell ref="C56:G56"/>
-    <mergeCell ref="I63:K63"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="B5:H5"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="F63:H63"/>
-    <mergeCell ref="B8:H8"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B47:H47"/>
-    <mergeCell ref="B62:H62"/>
-    <mergeCell ref="C48:G48"/>
-    <mergeCell ref="C49:G49"/>
-    <mergeCell ref="C50:G50"/>
-    <mergeCell ref="C51:G51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>